<commit_message>
add auth api and add department column
</commit_message>
<xml_diff>
--- a/public/templates/devices.xlsx
+++ b/public/templates/devices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CEED\PuestosVotacion\DeviceCheck\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29FCD67-2DDF-4812-BAE1-2A8C0CA288C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276310F-C89F-4FD0-8A9E-8AAC1B05D122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{51C2F127-5EDE-4C4C-B876-33722442B3BF}"/>
+    <workbookView xWindow="-24120" yWindow="840" windowWidth="24240" windowHeight="13020" xr2:uid="{51C2F127-5EDE-4C4C-B876-33722442B3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="176">
   <si>
     <t>id</t>
   </si>
@@ -54,31 +54,517 @@
     <t>consecutivo</t>
   </si>
   <si>
-    <t>0924ceb99d094936</t>
-  </si>
-  <si>
-    <t>188951196cc009a0</t>
-  </si>
-  <si>
-    <t>743bf032a915ba31</t>
-  </si>
-  <si>
-    <t>LLAVE12345</t>
-  </si>
-  <si>
-    <t>CONSECUTIVO12346</t>
-  </si>
-  <si>
-    <t>CONSECUTIVO12347</t>
-  </si>
-  <si>
-    <t>CONSECUTIVO12345</t>
-  </si>
-  <si>
-    <t>LLAVE12346</t>
-  </si>
-  <si>
-    <t>LLAVE12347</t>
+    <t>tel</t>
+  </si>
+  <si>
+    <t>08:00:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>09:00:00</t>
+  </si>
+  <si>
+    <t>a407935292005ba8</t>
+  </si>
+  <si>
+    <t>LLAVE1</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO1</t>
+  </si>
+  <si>
+    <t>2b3930f57cb1875f</t>
+  </si>
+  <si>
+    <t>LLAVE2</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO2</t>
+  </si>
+  <si>
+    <t>6ca4699753aee52e</t>
+  </si>
+  <si>
+    <t>LLAVE3</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO3</t>
+  </si>
+  <si>
+    <t>c729eb54b5445cd5</t>
+  </si>
+  <si>
+    <t>LLAVE4</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO4</t>
+  </si>
+  <si>
+    <t>3b117eea41fc35d3</t>
+  </si>
+  <si>
+    <t>LLAVE5</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO5</t>
+  </si>
+  <si>
+    <t>fc35cb344210ff42</t>
+  </si>
+  <si>
+    <t>LLAVE6</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO6</t>
+  </si>
+  <si>
+    <t>63efc1873a7981b4</t>
+  </si>
+  <si>
+    <t>LLAVE7</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO7</t>
+  </si>
+  <si>
+    <t>e721a2658fea85f6</t>
+  </si>
+  <si>
+    <t>LLAVE8</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO8</t>
+  </si>
+  <si>
+    <t>108262830fe7057a</t>
+  </si>
+  <si>
+    <t>LLAVE9</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO9</t>
+  </si>
+  <si>
+    <t>29269a207e9637dd</t>
+  </si>
+  <si>
+    <t>LLAVE10</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO10</t>
+  </si>
+  <si>
+    <t>17410f0359e28e34</t>
+  </si>
+  <si>
+    <t>LLAVE11</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO11</t>
+  </si>
+  <si>
+    <t>fedf550fb6c1ec83</t>
+  </si>
+  <si>
+    <t>LLAVE12</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO12</t>
+  </si>
+  <si>
+    <t>37781b56e84a018d</t>
+  </si>
+  <si>
+    <t>LLAVE13</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO13</t>
+  </si>
+  <si>
+    <t>b22a8cf74b996cd3</t>
+  </si>
+  <si>
+    <t>LLAVE14</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO14</t>
+  </si>
+  <si>
+    <t>1cc8911f5f940a33</t>
+  </si>
+  <si>
+    <t>LLAVE15</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO15</t>
+  </si>
+  <si>
+    <t>39e5909f43d7cd3d</t>
+  </si>
+  <si>
+    <t>LLAVE16</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO16</t>
+  </si>
+  <si>
+    <t>e8c19a8c48faa159</t>
+  </si>
+  <si>
+    <t>LLAVE17</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO17</t>
+  </si>
+  <si>
+    <t>6e9cb85db9a34279</t>
+  </si>
+  <si>
+    <t>LLAVE18</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO18</t>
+  </si>
+  <si>
+    <t>1b9dca59c9895d80</t>
+  </si>
+  <si>
+    <t>LLAVE19</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO19</t>
+  </si>
+  <si>
+    <t>860ed6bc87ee0bd2</t>
+  </si>
+  <si>
+    <t>LLAVE20</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO20</t>
+  </si>
+  <si>
+    <t>9af8e1e4be69ae57</t>
+  </si>
+  <si>
+    <t>LLAVE21</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO21</t>
+  </si>
+  <si>
+    <t>389d6a6df48c3d73</t>
+  </si>
+  <si>
+    <t>LLAVE22</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO22</t>
+  </si>
+  <si>
+    <t>8492221ddabd44bd</t>
+  </si>
+  <si>
+    <t>LLAVE23</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO23</t>
+  </si>
+  <si>
+    <t>d62deb5da8fa9991</t>
+  </si>
+  <si>
+    <t>LLAVE24</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO24</t>
+  </si>
+  <si>
+    <t>f3140d1099bc227b</t>
+  </si>
+  <si>
+    <t>LLAVE25</t>
+  </si>
+  <si>
+    <t>CONSECUTIVO25</t>
+  </si>
+  <si>
+    <t>08:00:01</t>
+  </si>
+  <si>
+    <t>09:00:01</t>
+  </si>
+  <si>
+    <t>10:00:01</t>
+  </si>
+  <si>
+    <t>08:00:02</t>
+  </si>
+  <si>
+    <t>09:00:02</t>
+  </si>
+  <si>
+    <t>10:00:02</t>
+  </si>
+  <si>
+    <t>08:00:03</t>
+  </si>
+  <si>
+    <t>09:00:03</t>
+  </si>
+  <si>
+    <t>10:00:03</t>
+  </si>
+  <si>
+    <t>08:00:04</t>
+  </si>
+  <si>
+    <t>09:00:04</t>
+  </si>
+  <si>
+    <t>10:00:04</t>
+  </si>
+  <si>
+    <t>08:00:05</t>
+  </si>
+  <si>
+    <t>09:00:05</t>
+  </si>
+  <si>
+    <t>10:00:05</t>
+  </si>
+  <si>
+    <t>08:00:06</t>
+  </si>
+  <si>
+    <t>09:00:06</t>
+  </si>
+  <si>
+    <t>10:00:06</t>
+  </si>
+  <si>
+    <t>08:00:07</t>
+  </si>
+  <si>
+    <t>09:00:07</t>
+  </si>
+  <si>
+    <t>10:00:07</t>
+  </si>
+  <si>
+    <t>08:00:08</t>
+  </si>
+  <si>
+    <t>latitud</t>
+  </si>
+  <si>
+    <t>longitud</t>
+  </si>
+  <si>
+    <t>7,0751600</t>
+  </si>
+  <si>
+    <t>-73,1686406</t>
+  </si>
+  <si>
+    <t>7,0751601</t>
+  </si>
+  <si>
+    <t>-73,1686407</t>
+  </si>
+  <si>
+    <t>7,0751602</t>
+  </si>
+  <si>
+    <t>-73,1686408</t>
+  </si>
+  <si>
+    <t>7,0751603</t>
+  </si>
+  <si>
+    <t>-73,1686409</t>
+  </si>
+  <si>
+    <t>7,0751604</t>
+  </si>
+  <si>
+    <t>-73,1686410</t>
+  </si>
+  <si>
+    <t>7,0751605</t>
+  </si>
+  <si>
+    <t>-73,1686411</t>
+  </si>
+  <si>
+    <t>7,0751606</t>
+  </si>
+  <si>
+    <t>-73,1686412</t>
+  </si>
+  <si>
+    <t>7,0751607</t>
+  </si>
+  <si>
+    <t>-73,1686413</t>
+  </si>
+  <si>
+    <t>7,0751608</t>
+  </si>
+  <si>
+    <t>-73,1686414</t>
+  </si>
+  <si>
+    <t>7,0751609</t>
+  </si>
+  <si>
+    <t>-73,1686415</t>
+  </si>
+  <si>
+    <t>7,0751610</t>
+  </si>
+  <si>
+    <t>-73,1686416</t>
+  </si>
+  <si>
+    <t>7,0751611</t>
+  </si>
+  <si>
+    <t>-73,1686417</t>
+  </si>
+  <si>
+    <t>7,0751612</t>
+  </si>
+  <si>
+    <t>-73,1686418</t>
+  </si>
+  <si>
+    <t>7,0751613</t>
+  </si>
+  <si>
+    <t>-73,1686419</t>
+  </si>
+  <si>
+    <t>7,0751614</t>
+  </si>
+  <si>
+    <t>-73,1686420</t>
+  </si>
+  <si>
+    <t>7,0751615</t>
+  </si>
+  <si>
+    <t>-73,1686421</t>
+  </si>
+  <si>
+    <t>7,0751616</t>
+  </si>
+  <si>
+    <t>-73,1686422</t>
+  </si>
+  <si>
+    <t>7,0751617</t>
+  </si>
+  <si>
+    <t>-73,1686423</t>
+  </si>
+  <si>
+    <t>7,0751618</t>
+  </si>
+  <si>
+    <t>-73,1686424</t>
+  </si>
+  <si>
+    <t>7,0751619</t>
+  </si>
+  <si>
+    <t>-73,1686425</t>
+  </si>
+  <si>
+    <t>7,0751620</t>
+  </si>
+  <si>
+    <t>-73,1686426</t>
+  </si>
+  <si>
+    <t>7,0751621</t>
+  </si>
+  <si>
+    <t>-73,1686427</t>
+  </si>
+  <si>
+    <t>7,0751622</t>
+  </si>
+  <si>
+    <t>-73,1686428</t>
+  </si>
+  <si>
+    <t>7,0751623</t>
+  </si>
+  <si>
+    <t>-73,1686429</t>
+  </si>
+  <si>
+    <t>llegada</t>
+  </si>
+  <si>
+    <t>salida</t>
+  </si>
+  <si>
+    <t>17:00:00</t>
+  </si>
+  <si>
+    <t>16:00:00</t>
+  </si>
+  <si>
+    <t>16:00:01</t>
+  </si>
+  <si>
+    <t>17:00:01</t>
+  </si>
+  <si>
+    <t>16:00:02</t>
+  </si>
+  <si>
+    <t>17:00:02</t>
+  </si>
+  <si>
+    <t>16:00:03</t>
+  </si>
+  <si>
+    <t>17:00:03</t>
+  </si>
+  <si>
+    <t>16:00:04</t>
+  </si>
+  <si>
+    <t>17:00:04</t>
+  </si>
+  <si>
+    <t>16:00:05</t>
+  </si>
+  <si>
+    <t>17:00:05</t>
+  </si>
+  <si>
+    <t>16:00:06</t>
+  </si>
+  <si>
+    <t>17:00:06</t>
+  </si>
+  <si>
+    <t>16:00:07</t>
+  </si>
+  <si>
+    <t>17:00:07</t>
+  </si>
+  <si>
+    <t>16:00:08</t>
+  </si>
+  <si>
+    <t>usuario_asignado</t>
   </si>
 </sst>
 </file>
@@ -120,8 +606,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,22 +923,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0A6A68-9E46-4463-AF34-E681701E16B3}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="K2" sqref="K2:K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,64 +949,837 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H1" t="s">
+        <v>157</v>
+      </c>
+      <c r="I1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>5</v>
+      <c r="C2">
+        <v>3152560926</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I2" s="1">
+        <v>7.0751599000000001</v>
+      </c>
+      <c r="J2" s="1">
+        <v>-73.168640499999995</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>3042773321</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>3234567891</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>3234567892</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>3234567893</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>3234567894</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C8">
+        <v>3234567895</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3234567896</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>3234567897</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3234567898</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>3234567899</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>3234567900</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>10</v>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>3234567901</v>
+      </c>
+      <c r="D14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>3234567902</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>3234567903</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>52</v>
+      </c>
+      <c r="F16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>3234567904</v>
+      </c>
+      <c r="D17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>3234567905</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>3234567906</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F19" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>3234567907</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+      <c r="F20" t="s">
+        <v>65</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>3234567908</v>
+      </c>
+      <c r="D21" t="s">
+        <v>66</v>
+      </c>
+      <c r="E21" t="s">
+        <v>67</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>3234567909</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>3234567910</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" t="s">
+        <v>74</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24">
+        <v>3234567911</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>3234567912</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26">
+        <v>3234567913</v>
+      </c>
+      <c r="D26" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F26" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change divipole asigned users
</commit_message>
<xml_diff>
--- a/public/templates/devices.xlsx
+++ b/public/templates/devices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CEED\PuestosVotacion\DeviceCheck\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3276310F-C89F-4FD0-8A9E-8AAC1B05D122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95925899-8F2D-4A54-AD54-74EB2C0EFAC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="840" windowWidth="24240" windowHeight="13020" xr2:uid="{51C2F127-5EDE-4C4C-B876-33722442B3BF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{51C2F127-5EDE-4C4C-B876-33722442B3BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
     <t>16:00:08</t>
   </si>
   <si>
-    <t>usuario_asignado</t>
+    <t>esbackup</t>
   </si>
 </sst>
 </file>
@@ -606,9 +606,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -926,7 +927,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K3"/>
+      <selection activeCell="K2" sqref="K2:K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1008,7 @@
       <c r="J2" s="1">
         <v>-73.168640499999995</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1042,8 +1043,8 @@
       <c r="J3" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K3">
-        <v>2</v>
+      <c r="K3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1077,6 +1078,9 @@
       <c r="J4" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1109,6 +1113,9 @@
       <c r="J5" s="1" t="s">
         <v>113</v>
       </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1141,6 +1148,9 @@
       <c r="J6" s="1" t="s">
         <v>115</v>
       </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1173,6 +1183,9 @@
       <c r="J7" s="1" t="s">
         <v>117</v>
       </c>
+      <c r="K7" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1205,6 +1218,9 @@
       <c r="J8" s="1" t="s">
         <v>119</v>
       </c>
+      <c r="K8" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1237,6 +1253,9 @@
       <c r="J9" s="1" t="s">
         <v>121</v>
       </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1269,6 +1288,9 @@
       <c r="J10" s="1" t="s">
         <v>123</v>
       </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1301,6 +1323,9 @@
       <c r="J11" s="1" t="s">
         <v>125</v>
       </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1333,6 +1358,9 @@
       <c r="J12" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="K12" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1365,6 +1393,9 @@
       <c r="J13" s="1" t="s">
         <v>129</v>
       </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1397,6 +1428,9 @@
       <c r="J14" s="1" t="s">
         <v>131</v>
       </c>
+      <c r="K14" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1429,6 +1463,9 @@
       <c r="J15" s="1" t="s">
         <v>133</v>
       </c>
+      <c r="K15" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1461,8 +1498,11 @@
       <c r="J16" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1493,8 +1533,11 @@
       <c r="J17" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1525,8 +1568,11 @@
       <c r="J18" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1557,8 +1603,11 @@
       <c r="J19" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1589,8 +1638,11 @@
       <c r="J20" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1621,8 +1673,11 @@
       <c r="J21" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1653,8 +1708,11 @@
       <c r="J22" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1685,8 +1743,11 @@
       <c r="J23" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1717,8 +1778,11 @@
       <c r="J24" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1749,8 +1813,11 @@
       <c r="J25" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1780,6 +1847,9 @@
       </c>
       <c r="J26" s="1" t="s">
         <v>155</v>
+      </c>
+      <c r="K26" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>